<commit_message>
Fixed excel bug. Added user headers list. Added code for headers and added syntax.
</commit_message>
<xml_diff>
--- a/Loadshedding.xlsx
+++ b/Loadshedding.xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25630"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{242F136E-8CB4-4E35-BCDD-2D4310D8286E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AEverything\Things on Deksktop\Python_now\Loadshedding_Google_Calendar\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Stage_1" sheetId="1" r:id="rId1"/>
@@ -17,7 +21,7 @@
     <sheet name="Stage_7" sheetId="7" r:id="rId7"/>
     <sheet name="Stage_8" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -138,11 +142,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,14 +183,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,19 +507,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -551,108 +558,108 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.10416666666666667</v>
       </c>
       <c r="C3" s="1"/>
@@ -663,11 +670,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.1875</v>
       </c>
       <c r="C4" s="1">
@@ -677,11 +684,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>0.27083333333333331</v>
       </c>
       <c r="P5" s="1">
@@ -691,11 +698,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.25</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0.35416666666666669</v>
       </c>
       <c r="L6" s="1">
@@ -705,11 +712,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>0.4375</v>
       </c>
       <c r="H7" s="1">
@@ -719,16 +726,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>1</v>
       </c>
@@ -736,22 +741,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>0.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>0.60416666666666663</v>
       </c>
       <c r="Q9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>0.6875</v>
       </c>
       <c r="M10" s="1">
@@ -761,11 +766,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="I11" s="1">
@@ -775,11 +780,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>0.75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>0.85416666666666663</v>
       </c>
       <c r="E12" s="1">
@@ -789,11 +794,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>0.9375</v>
       </c>
       <c r="R13" s="1">
@@ -803,11 +808,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
-      <c r="A14" s="3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="N14" s="1">
@@ -827,19 +832,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFBF558-A020-4020-B619-825AA55EE126}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -878,108 +883,108 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.10416666666666667</v>
       </c>
       <c r="C3" s="1"/>
@@ -1022,11 +1027,11 @@
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.1875</v>
       </c>
       <c r="C4" s="1">
@@ -1069,11 +1074,11 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>0.27083333333333331</v>
       </c>
       <c r="C5" s="1"/>
@@ -1114,11 +1119,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.25</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0.35416666666666669</v>
       </c>
       <c r="C6" s="1"/>
@@ -1161,11 +1166,11 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>0.4375</v>
       </c>
       <c r="C7" s="1"/>
@@ -1208,16 +1213,14 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>2</v>
       </c>
@@ -1257,11 +1260,11 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>0.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>0.60416666666666663</v>
       </c>
       <c r="C9" s="1"/>
@@ -1302,11 +1305,11 @@
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>0.6875</v>
       </c>
       <c r="C10" s="1"/>
@@ -1349,11 +1352,11 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="C11" s="1"/>
@@ -1396,11 +1399,11 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>0.75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>0.85416666666666663</v>
       </c>
       <c r="C12" s="1"/>
@@ -1443,11 +1446,11 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>0.9375</v>
       </c>
       <c r="C13" s="1"/>
@@ -1490,11 +1493,11 @@
       </c>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:33">
-      <c r="A14" s="3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C14" s="1"/>
@@ -1547,19 +1550,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6A537D-D09F-42F9-A62C-E3597CA0B7A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1598,108 +1601,108 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.10416666666666667</v>
       </c>
       <c r="C3" s="1"/>
@@ -1746,11 +1749,11 @@
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.1875</v>
       </c>
       <c r="C4" s="1">
@@ -1797,11 +1800,11 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>0.27083333333333331</v>
       </c>
       <c r="C5" s="1"/>
@@ -1846,11 +1849,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.25</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0.35416666666666669</v>
       </c>
       <c r="C6" s="1"/>
@@ -1897,11 +1900,11 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>0.4375</v>
       </c>
       <c r="C7" s="1"/>
@@ -1948,16 +1951,14 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C8" s="1">
-        <v>3</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>3</v>
       </c>
@@ -2001,11 +2002,11 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>0.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>0.60416666666666663</v>
       </c>
       <c r="C9" s="1"/>
@@ -2050,11 +2051,11 @@
       </c>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>0.6875</v>
       </c>
       <c r="C10" s="1"/>
@@ -2101,11 +2102,11 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="C11" s="1"/>
@@ -2152,11 +2153,11 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>0.75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>0.85416666666666663</v>
       </c>
       <c r="C12" s="1">
@@ -2203,11 +2204,11 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>0.9375</v>
       </c>
       <c r="C13" s="1"/>
@@ -2254,11 +2255,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
-      <c r="A14" s="3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C14" s="1"/>
@@ -2311,23 +2312,24 @@
     <mergeCell ref="C1:AG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8BBDA1-E175-4C2E-B0A8-26E5C0193FEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2366,108 +2368,108 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.10416666666666667</v>
       </c>
       <c r="C3" s="1"/>
@@ -2518,11 +2520,11 @@
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.1875</v>
       </c>
       <c r="C4" s="1">
@@ -2573,11 +2575,11 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>0.27083333333333331</v>
       </c>
       <c r="C5" s="1"/>
@@ -2626,11 +2628,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.25</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0.35416666666666669</v>
       </c>
       <c r="C6" s="1"/>
@@ -2681,11 +2683,11 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>0.4375</v>
       </c>
       <c r="C7" s="1"/>
@@ -2736,11 +2738,11 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>0.52083333333333337</v>
       </c>
       <c r="C8" s="1">
@@ -2791,11 +2793,11 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>0.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>0.60416666666666663</v>
       </c>
       <c r="C9" s="1"/>
@@ -2844,11 +2846,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>0.6875</v>
       </c>
       <c r="C10" s="1"/>
@@ -2899,11 +2901,11 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="C11" s="1"/>
@@ -2954,11 +2956,11 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>0.75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>0.85416666666666663</v>
       </c>
       <c r="C12" s="1">
@@ -3009,11 +3011,11 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>0.9375</v>
       </c>
       <c r="C13" s="1"/>
@@ -3062,11 +3064,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
-      <c r="A14" s="3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C14" s="1"/>
@@ -3127,19 +3129,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBC417B-AD57-4E8A-ABA3-6617FBFD7DC1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:AG14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3178,108 +3180,108 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.10416666666666667</v>
       </c>
       <c r="C3" s="1"/>
@@ -3334,11 +3336,11 @@
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.1875</v>
       </c>
       <c r="C4" s="1">
@@ -3393,11 +3395,11 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>0.27083333333333331</v>
       </c>
       <c r="C5" s="1">
@@ -3450,11 +3452,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.25</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0.35416666666666669</v>
       </c>
       <c r="C6" s="1"/>
@@ -3509,11 +3511,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>0.4375</v>
       </c>
       <c r="C7" s="1"/>
@@ -3568,11 +3570,11 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>0.52083333333333337</v>
       </c>
       <c r="C8" s="1">
@@ -3627,16 +3629,14 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>0.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>0.60416666666666663</v>
       </c>
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>5</v>
       </c>
@@ -3686,11 +3686,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>0.6875</v>
       </c>
       <c r="C10" s="1"/>
@@ -3743,11 +3743,11 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="C11" s="1"/>
@@ -3802,11 +3802,11 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>0.75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>0.85416666666666663</v>
       </c>
       <c r="C12" s="1">
@@ -3861,11 +3861,11 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>0.9375</v>
       </c>
       <c r="C13" s="1"/>
@@ -3918,11 +3918,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
-      <c r="A14" s="3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C14" s="1"/>
@@ -3987,19 +3987,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E6CB72-459A-411E-8C75-C3BACD5C6FCF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4038,108 +4038,108 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.10416666666666667</v>
       </c>
       <c r="G3" s="2">
@@ -4149,12 +4149,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.1875</v>
+      </c>
+      <c r="C4" s="4">
+        <v>6</v>
       </c>
       <c r="G4" s="1">
         <v>6</v>
@@ -4163,27 +4166,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>0.27083333333333331</v>
       </c>
-    </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="3">
+      <c r="C5" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.25</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0.35416666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>0.4375</v>
       </c>
       <c r="G7" s="1">
@@ -4193,38 +4199,41 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>0.52083333333333337</v>
+      </c>
+      <c r="C8" s="4">
+        <v>6</v>
       </c>
       <c r="H8" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>0.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>0.6875</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="G11" s="1">
@@ -4234,27 +4243,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>0.75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>0.85416666666666663</v>
       </c>
-    </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="3">
+      <c r="C12" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>0.9375</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
-      <c r="A14" s="3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
@@ -4268,19 +4280,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38A13F6-D5F0-40B8-97D8-018E3C308330}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4319,108 +4331,108 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.10416666666666667</v>
       </c>
       <c r="G3" s="2">
@@ -4430,11 +4442,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.1875</v>
       </c>
       <c r="G4" s="1">
@@ -4444,27 +4456,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>0.27083333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.25</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0.35416666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>0.4375</v>
       </c>
       <c r="G7" s="1">
@@ -4474,38 +4486,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>0.52083333333333337</v>
       </c>
       <c r="H8" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>0.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>0.6875</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="G11" s="1">
@@ -4515,30 +4527,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>0.75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>0.85416666666666663</v>
       </c>
       <c r="G12" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>0.9375</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
-      <c r="A14" s="3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
@@ -4552,19 +4564,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12012271-8F17-4692-B20D-5892FF866F38}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4603,108 +4615,108 @@
       <c r="AF1" s="6"/>
       <c r="AG1" s="6"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.10416666666666667</v>
       </c>
       <c r="G3" s="2">
@@ -4714,11 +4726,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.1875</v>
       </c>
       <c r="G4" s="1">
@@ -4728,27 +4740,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>0.27083333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>0.25</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0.35416666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>0.4375</v>
       </c>
       <c r="G7" s="1">
@@ -4758,11 +4770,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>0.52083333333333337</v>
       </c>
       <c r="G8" s="1">
@@ -4772,27 +4784,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>0.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>0.6875</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="G11" s="1">
@@ -4802,11 +4814,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>0.75</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>0.85416666666666663</v>
       </c>
       <c r="G12" s="1">
@@ -4816,19 +4828,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>0.9375</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
-      <c r="A14" s="3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>

</xml_diff>